<commit_message>
copy template row height
</commit_message>
<xml_diff>
--- a/src/test/resources/cepingtmpl.xlsx
+++ b/src/test/resources/cepingtmpl.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bingoobjca/go/src/github.com/bingoohuang/excel2javabeans/src/test/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{668E6031-B5BF-2C40-A553-EC644D09F1C0}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEC7EC8D-2CA3-1D41-BFB5-BC5BF5445C3C}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2093,6 +2093,54 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="1" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="1" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="11" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -2109,54 +2157,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="15" borderId="1" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="1" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="1" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -5025,7 +5025,7 @@
       <c r="F5" s="56"/>
       <c r="G5" s="57"/>
     </row>
-    <row r="6" spans="1:7" s="46" customFormat="1" ht="24" customHeight="1">
+    <row r="6" spans="1:7" s="46" customFormat="1" ht="58" customHeight="1">
       <c r="A6" s="47"/>
       <c r="B6" s="36" t="s">
         <v>17</v>
@@ -5257,16 +5257,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="A6:G6"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="D7:E7"/>
+    <mergeCell ref="A4:A5"/>
+    <mergeCell ref="B4:B5"/>
     <mergeCell ref="A1:G1"/>
     <mergeCell ref="C2:D2"/>
     <mergeCell ref="C3:D3"/>
     <mergeCell ref="C4:G4"/>
     <mergeCell ref="C5:G5"/>
-    <mergeCell ref="A6:G6"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="D7:E7"/>
-    <mergeCell ref="A4:A5"/>
-    <mergeCell ref="B4:B5"/>
   </mergeCells>
   <phoneticPr fontId="14" type="noConversion"/>
   <printOptions horizontalCentered="1" gridLines="1"/>
@@ -5489,289 +5489,289 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:273" s="3" customFormat="1" ht="13.5" customHeight="1">
-      <c r="A1" s="78" t="s">
+      <c r="A1" s="63" t="s">
         <v>29</v>
       </c>
-      <c r="B1" s="78"/>
-      <c r="C1" s="78"/>
-      <c r="D1" s="78"/>
-      <c r="E1" s="79" t="s">
+      <c r="B1" s="63"/>
+      <c r="C1" s="63"/>
+      <c r="D1" s="63"/>
+      <c r="E1" s="64" t="s">
         <v>30</v>
       </c>
-      <c r="F1" s="79"/>
-      <c r="G1" s="79"/>
-      <c r="H1" s="79"/>
-      <c r="I1" s="80" t="s">
+      <c r="F1" s="64"/>
+      <c r="G1" s="64"/>
+      <c r="H1" s="64"/>
+      <c r="I1" s="65" t="s">
         <v>31</v>
       </c>
-      <c r="J1" s="80"/>
-      <c r="K1" s="80"/>
-      <c r="L1" s="80"/>
-      <c r="M1" s="80"/>
-      <c r="N1" s="80"/>
-      <c r="O1" s="80"/>
-      <c r="P1" s="80"/>
-      <c r="Q1" s="80"/>
-      <c r="R1" s="80"/>
-      <c r="S1" s="80"/>
-      <c r="T1" s="80"/>
-      <c r="U1" s="80"/>
-      <c r="V1" s="80"/>
-      <c r="W1" s="80"/>
-      <c r="X1" s="80"/>
-      <c r="Y1" s="80"/>
-      <c r="Z1" s="80"/>
-      <c r="AA1" s="80"/>
-      <c r="AB1" s="80"/>
-      <c r="AC1" s="80"/>
-      <c r="AD1" s="80"/>
-      <c r="AE1" s="80"/>
-      <c r="AF1" s="80"/>
-      <c r="AG1" s="80"/>
-      <c r="AH1" s="80"/>
-      <c r="AI1" s="80"/>
-      <c r="AJ1" s="80"/>
-      <c r="AK1" s="80"/>
-      <c r="AL1" s="80"/>
-      <c r="AM1" s="80"/>
-      <c r="AN1" s="81" t="s">
+      <c r="J1" s="65"/>
+      <c r="K1" s="65"/>
+      <c r="L1" s="65"/>
+      <c r="M1" s="65"/>
+      <c r="N1" s="65"/>
+      <c r="O1" s="65"/>
+      <c r="P1" s="65"/>
+      <c r="Q1" s="65"/>
+      <c r="R1" s="65"/>
+      <c r="S1" s="65"/>
+      <c r="T1" s="65"/>
+      <c r="U1" s="65"/>
+      <c r="V1" s="65"/>
+      <c r="W1" s="65"/>
+      <c r="X1" s="65"/>
+      <c r="Y1" s="65"/>
+      <c r="Z1" s="65"/>
+      <c r="AA1" s="65"/>
+      <c r="AB1" s="65"/>
+      <c r="AC1" s="65"/>
+      <c r="AD1" s="65"/>
+      <c r="AE1" s="65"/>
+      <c r="AF1" s="65"/>
+      <c r="AG1" s="65"/>
+      <c r="AH1" s="65"/>
+      <c r="AI1" s="65"/>
+      <c r="AJ1" s="65"/>
+      <c r="AK1" s="65"/>
+      <c r="AL1" s="65"/>
+      <c r="AM1" s="65"/>
+      <c r="AN1" s="66" t="s">
         <v>32</v>
       </c>
-      <c r="AO1" s="82"/>
-      <c r="AP1" s="82"/>
-      <c r="AQ1" s="82"/>
-      <c r="AR1" s="82"/>
-      <c r="AS1" s="82"/>
-      <c r="AT1" s="82"/>
-      <c r="AU1" s="82"/>
-      <c r="AV1" s="82"/>
-      <c r="AW1" s="82"/>
-      <c r="AX1" s="82"/>
-      <c r="AY1" s="82"/>
-      <c r="AZ1" s="82"/>
-      <c r="BA1" s="82"/>
-      <c r="BB1" s="82"/>
-      <c r="BC1" s="82"/>
-      <c r="BD1" s="82"/>
-      <c r="BE1" s="82"/>
-      <c r="BF1" s="82"/>
-      <c r="BG1" s="82"/>
-      <c r="BH1" s="82"/>
-      <c r="BI1" s="82"/>
-      <c r="BJ1" s="82"/>
-      <c r="BK1" s="82"/>
-      <c r="BL1" s="82"/>
-      <c r="BM1" s="83"/>
-      <c r="BN1" s="84" t="s">
+      <c r="AO1" s="67"/>
+      <c r="AP1" s="67"/>
+      <c r="AQ1" s="67"/>
+      <c r="AR1" s="67"/>
+      <c r="AS1" s="67"/>
+      <c r="AT1" s="67"/>
+      <c r="AU1" s="67"/>
+      <c r="AV1" s="67"/>
+      <c r="AW1" s="67"/>
+      <c r="AX1" s="67"/>
+      <c r="AY1" s="67"/>
+      <c r="AZ1" s="67"/>
+      <c r="BA1" s="67"/>
+      <c r="BB1" s="67"/>
+      <c r="BC1" s="67"/>
+      <c r="BD1" s="67"/>
+      <c r="BE1" s="67"/>
+      <c r="BF1" s="67"/>
+      <c r="BG1" s="67"/>
+      <c r="BH1" s="67"/>
+      <c r="BI1" s="67"/>
+      <c r="BJ1" s="67"/>
+      <c r="BK1" s="67"/>
+      <c r="BL1" s="67"/>
+      <c r="BM1" s="68"/>
+      <c r="BN1" s="69" t="s">
         <v>33</v>
       </c>
-      <c r="BO1" s="84"/>
-      <c r="BP1" s="84"/>
-      <c r="BQ1" s="84"/>
-      <c r="BR1" s="84"/>
-      <c r="BS1" s="84"/>
-      <c r="BT1" s="84"/>
-      <c r="BU1" s="84"/>
-      <c r="BV1" s="84"/>
-      <c r="BW1" s="84"/>
-      <c r="BX1" s="84"/>
-      <c r="BY1" s="84"/>
-      <c r="BZ1" s="84"/>
-      <c r="CA1" s="84"/>
-      <c r="CB1" s="84"/>
-      <c r="CC1" s="84"/>
-      <c r="CD1" s="84"/>
-      <c r="CE1" s="84"/>
-      <c r="CF1" s="84"/>
-      <c r="CG1" s="84"/>
-      <c r="CH1" s="84"/>
-      <c r="CI1" s="84"/>
-      <c r="CJ1" s="84"/>
-      <c r="CK1" s="84"/>
-      <c r="CL1" s="84"/>
-      <c r="CM1" s="84"/>
-      <c r="CN1" s="84"/>
-      <c r="CO1" s="84"/>
-      <c r="CP1" s="84"/>
-      <c r="CQ1" s="84"/>
-      <c r="CR1" s="84"/>
-      <c r="CS1" s="84"/>
-      <c r="CT1" s="84"/>
-      <c r="CU1" s="84"/>
-      <c r="CV1" s="84"/>
-      <c r="CW1" s="84"/>
-      <c r="CX1" s="84"/>
-      <c r="CY1" s="84"/>
-      <c r="CZ1" s="84"/>
-      <c r="DA1" s="84"/>
-      <c r="DB1" s="84"/>
-      <c r="DC1" s="84"/>
-      <c r="DD1" s="84"/>
-      <c r="DE1" s="84"/>
-      <c r="DF1" s="84"/>
-      <c r="DG1" s="84"/>
-      <c r="DH1" s="84"/>
-      <c r="DI1" s="84"/>
-      <c r="DJ1" s="84"/>
-      <c r="DK1" s="84"/>
-      <c r="DL1" s="84"/>
-      <c r="DM1" s="84"/>
-      <c r="DN1" s="84"/>
-      <c r="DO1" s="84"/>
-      <c r="DP1" s="84"/>
-      <c r="DQ1" s="84"/>
-      <c r="DR1" s="84"/>
-      <c r="DS1" s="84"/>
-      <c r="DT1" s="84"/>
-      <c r="DU1" s="84"/>
-      <c r="DV1" s="84"/>
-      <c r="DW1" s="84"/>
-      <c r="DX1" s="84"/>
-      <c r="DY1" s="84"/>
-      <c r="DZ1" s="84"/>
-      <c r="EA1" s="84"/>
-      <c r="EB1" s="84"/>
-      <c r="EC1" s="84"/>
-      <c r="ED1" s="84"/>
-      <c r="EE1" s="84"/>
-      <c r="EF1" s="84"/>
-      <c r="EG1" s="84"/>
-      <c r="EH1" s="84"/>
-      <c r="EI1" s="84"/>
-      <c r="EJ1" s="84"/>
-      <c r="EK1" s="84"/>
-      <c r="EL1" s="84"/>
-      <c r="EM1" s="84"/>
-      <c r="EN1" s="84"/>
-      <c r="EO1" s="84"/>
-      <c r="EP1" s="84"/>
-      <c r="EQ1" s="84"/>
-      <c r="ER1" s="84"/>
-      <c r="ES1" s="84"/>
-      <c r="ET1" s="84"/>
-      <c r="EU1" s="84"/>
-      <c r="EV1" s="84"/>
-      <c r="EW1" s="84"/>
-      <c r="EX1" s="84"/>
-      <c r="EY1" s="84"/>
-      <c r="EZ1" s="84"/>
-      <c r="FA1" s="84"/>
-      <c r="FB1" s="84"/>
-      <c r="FC1" s="84"/>
-      <c r="FD1" s="84"/>
-      <c r="FE1" s="84"/>
-      <c r="FF1" s="84"/>
-      <c r="FG1" s="84"/>
-      <c r="FH1" s="84"/>
-      <c r="FI1" s="84"/>
-      <c r="FJ1" s="84"/>
-      <c r="FK1" s="84"/>
-      <c r="FL1" s="84"/>
-      <c r="FM1" s="84"/>
-      <c r="FN1" s="84"/>
-      <c r="FO1" s="84"/>
-      <c r="FP1" s="84"/>
-      <c r="FQ1" s="84"/>
-      <c r="FR1" s="84"/>
-      <c r="FS1" s="84"/>
-      <c r="FT1" s="84"/>
-      <c r="FU1" s="84"/>
-      <c r="FV1" s="84"/>
-      <c r="FW1" s="84"/>
-      <c r="FX1" s="84"/>
-      <c r="FY1" s="84"/>
-      <c r="FZ1" s="84"/>
-      <c r="GA1" s="84"/>
-      <c r="GB1" s="84"/>
-      <c r="GC1" s="84"/>
-      <c r="GD1" s="84"/>
-      <c r="GE1" s="84"/>
-      <c r="GF1" s="84"/>
-      <c r="GG1" s="84"/>
-      <c r="GH1" s="84"/>
-      <c r="GI1" s="84"/>
-      <c r="GJ1" s="84"/>
-      <c r="GK1" s="84"/>
-      <c r="GL1" s="84"/>
-      <c r="GM1" s="84"/>
-      <c r="GN1" s="84"/>
-      <c r="GO1" s="84"/>
-      <c r="GP1" s="84"/>
-      <c r="GQ1" s="84"/>
-      <c r="GR1" s="84"/>
-      <c r="GS1" s="84"/>
-      <c r="GT1" s="84"/>
-      <c r="GU1" s="84"/>
-      <c r="GV1" s="84"/>
-      <c r="GW1" s="84"/>
-      <c r="GX1" s="84"/>
-      <c r="GY1" s="84"/>
-      <c r="GZ1" s="84"/>
-      <c r="HA1" s="84"/>
-      <c r="HB1" s="84"/>
-      <c r="HC1" s="84"/>
-      <c r="HD1" s="84"/>
-      <c r="HE1" s="84"/>
-      <c r="HF1" s="84"/>
-      <c r="HG1" s="84"/>
-      <c r="HH1" s="84"/>
-      <c r="HI1" s="84"/>
-      <c r="HJ1" s="84"/>
-      <c r="HK1" s="84"/>
-      <c r="HL1" s="84"/>
-      <c r="HM1" s="84"/>
-      <c r="HN1" s="84"/>
-      <c r="HO1" s="84"/>
-      <c r="HP1" s="84"/>
-      <c r="HQ1" s="84"/>
-      <c r="HR1" s="84"/>
-      <c r="HS1" s="84"/>
-      <c r="HT1" s="84"/>
-      <c r="HU1" s="84"/>
-      <c r="HV1" s="84"/>
-      <c r="HW1" s="84"/>
-      <c r="HX1" s="84"/>
-      <c r="HY1" s="84"/>
-      <c r="HZ1" s="84"/>
-      <c r="IA1" s="84"/>
-      <c r="IB1" s="84"/>
-      <c r="IC1" s="84"/>
-      <c r="ID1" s="84"/>
-      <c r="IE1" s="84"/>
-      <c r="IF1" s="84"/>
-      <c r="IG1" s="84"/>
-      <c r="IH1" s="84"/>
-      <c r="II1" s="84"/>
-      <c r="IJ1" s="84"/>
-      <c r="IK1" s="84"/>
-      <c r="IL1" s="84"/>
-      <c r="IM1" s="84"/>
-      <c r="IN1" s="84"/>
-      <c r="IO1" s="84"/>
-      <c r="IP1" s="84"/>
-      <c r="IQ1" s="84"/>
-      <c r="IR1" s="84"/>
-      <c r="IS1" s="84"/>
-      <c r="IT1" s="84"/>
-      <c r="IU1" s="84"/>
-      <c r="IV1" s="84"/>
-      <c r="IW1" s="84"/>
-      <c r="IX1" s="84"/>
-      <c r="IY1" s="84"/>
-      <c r="IZ1" s="84"/>
-      <c r="JA1" s="84"/>
-      <c r="JB1" s="84"/>
-      <c r="JC1" s="84"/>
-      <c r="JD1" s="84"/>
-      <c r="JE1" s="84"/>
-      <c r="JF1" s="84"/>
-      <c r="JG1" s="84"/>
-      <c r="JH1" s="84"/>
-      <c r="JI1" s="84"/>
-      <c r="JJ1" s="84"/>
-      <c r="JK1" s="84"/>
-      <c r="JL1" s="84"/>
-      <c r="JM1" s="84"/>
+      <c r="BO1" s="69"/>
+      <c r="BP1" s="69"/>
+      <c r="BQ1" s="69"/>
+      <c r="BR1" s="69"/>
+      <c r="BS1" s="69"/>
+      <c r="BT1" s="69"/>
+      <c r="BU1" s="69"/>
+      <c r="BV1" s="69"/>
+      <c r="BW1" s="69"/>
+      <c r="BX1" s="69"/>
+      <c r="BY1" s="69"/>
+      <c r="BZ1" s="69"/>
+      <c r="CA1" s="69"/>
+      <c r="CB1" s="69"/>
+      <c r="CC1" s="69"/>
+      <c r="CD1" s="69"/>
+      <c r="CE1" s="69"/>
+      <c r="CF1" s="69"/>
+      <c r="CG1" s="69"/>
+      <c r="CH1" s="69"/>
+      <c r="CI1" s="69"/>
+      <c r="CJ1" s="69"/>
+      <c r="CK1" s="69"/>
+      <c r="CL1" s="69"/>
+      <c r="CM1" s="69"/>
+      <c r="CN1" s="69"/>
+      <c r="CO1" s="69"/>
+      <c r="CP1" s="69"/>
+      <c r="CQ1" s="69"/>
+      <c r="CR1" s="69"/>
+      <c r="CS1" s="69"/>
+      <c r="CT1" s="69"/>
+      <c r="CU1" s="69"/>
+      <c r="CV1" s="69"/>
+      <c r="CW1" s="69"/>
+      <c r="CX1" s="69"/>
+      <c r="CY1" s="69"/>
+      <c r="CZ1" s="69"/>
+      <c r="DA1" s="69"/>
+      <c r="DB1" s="69"/>
+      <c r="DC1" s="69"/>
+      <c r="DD1" s="69"/>
+      <c r="DE1" s="69"/>
+      <c r="DF1" s="69"/>
+      <c r="DG1" s="69"/>
+      <c r="DH1" s="69"/>
+      <c r="DI1" s="69"/>
+      <c r="DJ1" s="69"/>
+      <c r="DK1" s="69"/>
+      <c r="DL1" s="69"/>
+      <c r="DM1" s="69"/>
+      <c r="DN1" s="69"/>
+      <c r="DO1" s="69"/>
+      <c r="DP1" s="69"/>
+      <c r="DQ1" s="69"/>
+      <c r="DR1" s="69"/>
+      <c r="DS1" s="69"/>
+      <c r="DT1" s="69"/>
+      <c r="DU1" s="69"/>
+      <c r="DV1" s="69"/>
+      <c r="DW1" s="69"/>
+      <c r="DX1" s="69"/>
+      <c r="DY1" s="69"/>
+      <c r="DZ1" s="69"/>
+      <c r="EA1" s="69"/>
+      <c r="EB1" s="69"/>
+      <c r="EC1" s="69"/>
+      <c r="ED1" s="69"/>
+      <c r="EE1" s="69"/>
+      <c r="EF1" s="69"/>
+      <c r="EG1" s="69"/>
+      <c r="EH1" s="69"/>
+      <c r="EI1" s="69"/>
+      <c r="EJ1" s="69"/>
+      <c r="EK1" s="69"/>
+      <c r="EL1" s="69"/>
+      <c r="EM1" s="69"/>
+      <c r="EN1" s="69"/>
+      <c r="EO1" s="69"/>
+      <c r="EP1" s="69"/>
+      <c r="EQ1" s="69"/>
+      <c r="ER1" s="69"/>
+      <c r="ES1" s="69"/>
+      <c r="ET1" s="69"/>
+      <c r="EU1" s="69"/>
+      <c r="EV1" s="69"/>
+      <c r="EW1" s="69"/>
+      <c r="EX1" s="69"/>
+      <c r="EY1" s="69"/>
+      <c r="EZ1" s="69"/>
+      <c r="FA1" s="69"/>
+      <c r="FB1" s="69"/>
+      <c r="FC1" s="69"/>
+      <c r="FD1" s="69"/>
+      <c r="FE1" s="69"/>
+      <c r="FF1" s="69"/>
+      <c r="FG1" s="69"/>
+      <c r="FH1" s="69"/>
+      <c r="FI1" s="69"/>
+      <c r="FJ1" s="69"/>
+      <c r="FK1" s="69"/>
+      <c r="FL1" s="69"/>
+      <c r="FM1" s="69"/>
+      <c r="FN1" s="69"/>
+      <c r="FO1" s="69"/>
+      <c r="FP1" s="69"/>
+      <c r="FQ1" s="69"/>
+      <c r="FR1" s="69"/>
+      <c r="FS1" s="69"/>
+      <c r="FT1" s="69"/>
+      <c r="FU1" s="69"/>
+      <c r="FV1" s="69"/>
+      <c r="FW1" s="69"/>
+      <c r="FX1" s="69"/>
+      <c r="FY1" s="69"/>
+      <c r="FZ1" s="69"/>
+      <c r="GA1" s="69"/>
+      <c r="GB1" s="69"/>
+      <c r="GC1" s="69"/>
+      <c r="GD1" s="69"/>
+      <c r="GE1" s="69"/>
+      <c r="GF1" s="69"/>
+      <c r="GG1" s="69"/>
+      <c r="GH1" s="69"/>
+      <c r="GI1" s="69"/>
+      <c r="GJ1" s="69"/>
+      <c r="GK1" s="69"/>
+      <c r="GL1" s="69"/>
+      <c r="GM1" s="69"/>
+      <c r="GN1" s="69"/>
+      <c r="GO1" s="69"/>
+      <c r="GP1" s="69"/>
+      <c r="GQ1" s="69"/>
+      <c r="GR1" s="69"/>
+      <c r="GS1" s="69"/>
+      <c r="GT1" s="69"/>
+      <c r="GU1" s="69"/>
+      <c r="GV1" s="69"/>
+      <c r="GW1" s="69"/>
+      <c r="GX1" s="69"/>
+      <c r="GY1" s="69"/>
+      <c r="GZ1" s="69"/>
+      <c r="HA1" s="69"/>
+      <c r="HB1" s="69"/>
+      <c r="HC1" s="69"/>
+      <c r="HD1" s="69"/>
+      <c r="HE1" s="69"/>
+      <c r="HF1" s="69"/>
+      <c r="HG1" s="69"/>
+      <c r="HH1" s="69"/>
+      <c r="HI1" s="69"/>
+      <c r="HJ1" s="69"/>
+      <c r="HK1" s="69"/>
+      <c r="HL1" s="69"/>
+      <c r="HM1" s="69"/>
+      <c r="HN1" s="69"/>
+      <c r="HO1" s="69"/>
+      <c r="HP1" s="69"/>
+      <c r="HQ1" s="69"/>
+      <c r="HR1" s="69"/>
+      <c r="HS1" s="69"/>
+      <c r="HT1" s="69"/>
+      <c r="HU1" s="69"/>
+      <c r="HV1" s="69"/>
+      <c r="HW1" s="69"/>
+      <c r="HX1" s="69"/>
+      <c r="HY1" s="69"/>
+      <c r="HZ1" s="69"/>
+      <c r="IA1" s="69"/>
+      <c r="IB1" s="69"/>
+      <c r="IC1" s="69"/>
+      <c r="ID1" s="69"/>
+      <c r="IE1" s="69"/>
+      <c r="IF1" s="69"/>
+      <c r="IG1" s="69"/>
+      <c r="IH1" s="69"/>
+      <c r="II1" s="69"/>
+      <c r="IJ1" s="69"/>
+      <c r="IK1" s="69"/>
+      <c r="IL1" s="69"/>
+      <c r="IM1" s="69"/>
+      <c r="IN1" s="69"/>
+      <c r="IO1" s="69"/>
+      <c r="IP1" s="69"/>
+      <c r="IQ1" s="69"/>
+      <c r="IR1" s="69"/>
+      <c r="IS1" s="69"/>
+      <c r="IT1" s="69"/>
+      <c r="IU1" s="69"/>
+      <c r="IV1" s="69"/>
+      <c r="IW1" s="69"/>
+      <c r="IX1" s="69"/>
+      <c r="IY1" s="69"/>
+      <c r="IZ1" s="69"/>
+      <c r="JA1" s="69"/>
+      <c r="JB1" s="69"/>
+      <c r="JC1" s="69"/>
+      <c r="JD1" s="69"/>
+      <c r="JE1" s="69"/>
+      <c r="JF1" s="69"/>
+      <c r="JG1" s="69"/>
+      <c r="JH1" s="69"/>
+      <c r="JI1" s="69"/>
+      <c r="JJ1" s="69"/>
+      <c r="JK1" s="69"/>
+      <c r="JL1" s="69"/>
+      <c r="JM1" s="69"/>
     </row>
     <row r="2" spans="1:273" s="3" customFormat="1" ht="40.5" customHeight="1">
       <c r="A2" s="8"/>
@@ -5782,303 +5782,303 @@
       <c r="F2" s="8"/>
       <c r="G2" s="8"/>
       <c r="H2" s="8"/>
-      <c r="I2" s="77" t="s">
+      <c r="I2" s="70" t="s">
         <v>34</v>
       </c>
-      <c r="J2" s="77"/>
-      <c r="K2" s="77"/>
-      <c r="L2" s="77"/>
-      <c r="M2" s="77"/>
-      <c r="N2" s="77"/>
-      <c r="O2" s="77"/>
-      <c r="P2" s="77"/>
-      <c r="Q2" s="77"/>
-      <c r="R2" s="77"/>
-      <c r="S2" s="77"/>
-      <c r="T2" s="77"/>
-      <c r="U2" s="77"/>
-      <c r="V2" s="77" t="s">
+      <c r="J2" s="70"/>
+      <c r="K2" s="70"/>
+      <c r="L2" s="70"/>
+      <c r="M2" s="70"/>
+      <c r="N2" s="70"/>
+      <c r="O2" s="70"/>
+      <c r="P2" s="70"/>
+      <c r="Q2" s="70"/>
+      <c r="R2" s="70"/>
+      <c r="S2" s="70"/>
+      <c r="T2" s="70"/>
+      <c r="U2" s="70"/>
+      <c r="V2" s="70" t="s">
         <v>35</v>
       </c>
-      <c r="W2" s="77"/>
-      <c r="X2" s="77"/>
-      <c r="Y2" s="77"/>
-      <c r="Z2" s="77"/>
-      <c r="AA2" s="77"/>
-      <c r="AB2" s="77"/>
-      <c r="AC2" s="77" t="s">
+      <c r="W2" s="70"/>
+      <c r="X2" s="70"/>
+      <c r="Y2" s="70"/>
+      <c r="Z2" s="70"/>
+      <c r="AA2" s="70"/>
+      <c r="AB2" s="70"/>
+      <c r="AC2" s="70" t="s">
         <v>36</v>
       </c>
-      <c r="AD2" s="77"/>
-      <c r="AE2" s="77"/>
-      <c r="AF2" s="77"/>
-      <c r="AG2" s="77"/>
-      <c r="AH2" s="77"/>
-      <c r="AI2" s="77" t="s">
+      <c r="AD2" s="70"/>
+      <c r="AE2" s="70"/>
+      <c r="AF2" s="70"/>
+      <c r="AG2" s="70"/>
+      <c r="AH2" s="70"/>
+      <c r="AI2" s="70" t="s">
         <v>37</v>
       </c>
-      <c r="AJ2" s="77"/>
-      <c r="AK2" s="77"/>
-      <c r="AL2" s="77"/>
-      <c r="AM2" s="77"/>
-      <c r="AN2" s="69" t="s">
+      <c r="AJ2" s="70"/>
+      <c r="AK2" s="70"/>
+      <c r="AL2" s="70"/>
+      <c r="AM2" s="70"/>
+      <c r="AN2" s="71" t="s">
         <v>38</v>
       </c>
-      <c r="AO2" s="70"/>
-      <c r="AP2" s="70"/>
-      <c r="AQ2" s="71"/>
-      <c r="AR2" s="69" t="s">
+      <c r="AO2" s="72"/>
+      <c r="AP2" s="72"/>
+      <c r="AQ2" s="73"/>
+      <c r="AR2" s="71" t="s">
         <v>39</v>
       </c>
-      <c r="AS2" s="70"/>
-      <c r="AT2" s="70"/>
-      <c r="AU2" s="70"/>
-      <c r="AV2" s="70"/>
-      <c r="AW2" s="70"/>
-      <c r="AX2" s="70"/>
-      <c r="AY2" s="70"/>
-      <c r="AZ2" s="70"/>
-      <c r="BA2" s="70"/>
-      <c r="BB2" s="70"/>
-      <c r="BC2" s="70"/>
-      <c r="BD2" s="70"/>
-      <c r="BE2" s="70"/>
-      <c r="BF2" s="70"/>
-      <c r="BG2" s="70"/>
-      <c r="BH2" s="70"/>
-      <c r="BI2" s="70"/>
-      <c r="BJ2" s="70"/>
-      <c r="BK2" s="70"/>
-      <c r="BL2" s="70"/>
-      <c r="BM2" s="71"/>
+      <c r="AS2" s="72"/>
+      <c r="AT2" s="72"/>
+      <c r="AU2" s="72"/>
+      <c r="AV2" s="72"/>
+      <c r="AW2" s="72"/>
+      <c r="AX2" s="72"/>
+      <c r="AY2" s="72"/>
+      <c r="AZ2" s="72"/>
+      <c r="BA2" s="72"/>
+      <c r="BB2" s="72"/>
+      <c r="BC2" s="72"/>
+      <c r="BD2" s="72"/>
+      <c r="BE2" s="72"/>
+      <c r="BF2" s="72"/>
+      <c r="BG2" s="72"/>
+      <c r="BH2" s="72"/>
+      <c r="BI2" s="72"/>
+      <c r="BJ2" s="72"/>
+      <c r="BK2" s="72"/>
+      <c r="BL2" s="72"/>
+      <c r="BM2" s="73"/>
       <c r="BN2" s="13" t="s">
         <v>40</v>
       </c>
-      <c r="BO2" s="72" t="s">
+      <c r="BO2" s="74" t="s">
         <v>41</v>
       </c>
-      <c r="BP2" s="73"/>
-      <c r="BQ2" s="73"/>
-      <c r="BR2" s="73"/>
-      <c r="BS2" s="73"/>
-      <c r="BT2" s="73"/>
-      <c r="BU2" s="73"/>
-      <c r="BV2" s="73"/>
-      <c r="BW2" s="73"/>
-      <c r="BX2" s="73"/>
-      <c r="BY2" s="73"/>
-      <c r="BZ2" s="73"/>
-      <c r="CA2" s="73"/>
-      <c r="CB2" s="73"/>
-      <c r="CC2" s="73"/>
-      <c r="CD2" s="73"/>
-      <c r="CE2" s="73"/>
-      <c r="CF2" s="73"/>
-      <c r="CG2" s="73"/>
-      <c r="CH2" s="73"/>
-      <c r="CI2" s="74" t="s">
+      <c r="BP2" s="75"/>
+      <c r="BQ2" s="75"/>
+      <c r="BR2" s="75"/>
+      <c r="BS2" s="75"/>
+      <c r="BT2" s="75"/>
+      <c r="BU2" s="75"/>
+      <c r="BV2" s="75"/>
+      <c r="BW2" s="75"/>
+      <c r="BX2" s="75"/>
+      <c r="BY2" s="75"/>
+      <c r="BZ2" s="75"/>
+      <c r="CA2" s="75"/>
+      <c r="CB2" s="75"/>
+      <c r="CC2" s="75"/>
+      <c r="CD2" s="75"/>
+      <c r="CE2" s="75"/>
+      <c r="CF2" s="75"/>
+      <c r="CG2" s="75"/>
+      <c r="CH2" s="75"/>
+      <c r="CI2" s="76" t="s">
         <v>42</v>
       </c>
-      <c r="CJ2" s="74"/>
-      <c r="CK2" s="74"/>
-      <c r="CL2" s="74"/>
-      <c r="CM2" s="74"/>
-      <c r="CN2" s="74"/>
-      <c r="CO2" s="74"/>
-      <c r="CP2" s="74"/>
-      <c r="CQ2" s="74"/>
-      <c r="CR2" s="74"/>
-      <c r="CS2" s="74"/>
-      <c r="CT2" s="74"/>
-      <c r="CU2" s="74"/>
-      <c r="CV2" s="74"/>
-      <c r="CW2" s="74"/>
-      <c r="CX2" s="74"/>
-      <c r="CY2" s="75" t="s">
+      <c r="CJ2" s="76"/>
+      <c r="CK2" s="76"/>
+      <c r="CL2" s="76"/>
+      <c r="CM2" s="76"/>
+      <c r="CN2" s="76"/>
+      <c r="CO2" s="76"/>
+      <c r="CP2" s="76"/>
+      <c r="CQ2" s="76"/>
+      <c r="CR2" s="76"/>
+      <c r="CS2" s="76"/>
+      <c r="CT2" s="76"/>
+      <c r="CU2" s="76"/>
+      <c r="CV2" s="76"/>
+      <c r="CW2" s="76"/>
+      <c r="CX2" s="76"/>
+      <c r="CY2" s="77" t="s">
         <v>43</v>
       </c>
-      <c r="CZ2" s="75"/>
-      <c r="DA2" s="75"/>
-      <c r="DB2" s="75"/>
-      <c r="DC2" s="75"/>
-      <c r="DD2" s="75"/>
-      <c r="DE2" s="75"/>
-      <c r="DF2" s="75"/>
-      <c r="DG2" s="75"/>
-      <c r="DH2" s="75"/>
-      <c r="DI2" s="75"/>
-      <c r="DJ2" s="76" t="s">
+      <c r="CZ2" s="77"/>
+      <c r="DA2" s="77"/>
+      <c r="DB2" s="77"/>
+      <c r="DC2" s="77"/>
+      <c r="DD2" s="77"/>
+      <c r="DE2" s="77"/>
+      <c r="DF2" s="77"/>
+      <c r="DG2" s="77"/>
+      <c r="DH2" s="77"/>
+      <c r="DI2" s="77"/>
+      <c r="DJ2" s="78" t="s">
         <v>44</v>
       </c>
-      <c r="DK2" s="76"/>
-      <c r="DL2" s="76"/>
-      <c r="DM2" s="76"/>
-      <c r="DN2" s="76"/>
-      <c r="DO2" s="76"/>
-      <c r="DP2" s="76"/>
-      <c r="DQ2" s="76"/>
-      <c r="DR2" s="76"/>
-      <c r="DS2" s="76"/>
-      <c r="DT2" s="76"/>
-      <c r="DU2" s="76"/>
-      <c r="DV2" s="76"/>
-      <c r="DW2" s="76"/>
-      <c r="DX2" s="76"/>
-      <c r="DY2" s="76"/>
-      <c r="DZ2" s="76"/>
-      <c r="EA2" s="76"/>
-      <c r="EB2" s="76"/>
-      <c r="EC2" s="76"/>
-      <c r="ED2" s="76"/>
-      <c r="EE2" s="63" t="s">
+      <c r="DK2" s="78"/>
+      <c r="DL2" s="78"/>
+      <c r="DM2" s="78"/>
+      <c r="DN2" s="78"/>
+      <c r="DO2" s="78"/>
+      <c r="DP2" s="78"/>
+      <c r="DQ2" s="78"/>
+      <c r="DR2" s="78"/>
+      <c r="DS2" s="78"/>
+      <c r="DT2" s="78"/>
+      <c r="DU2" s="78"/>
+      <c r="DV2" s="78"/>
+      <c r="DW2" s="78"/>
+      <c r="DX2" s="78"/>
+      <c r="DY2" s="78"/>
+      <c r="DZ2" s="78"/>
+      <c r="EA2" s="78"/>
+      <c r="EB2" s="78"/>
+      <c r="EC2" s="78"/>
+      <c r="ED2" s="78"/>
+      <c r="EE2" s="79" t="s">
         <v>45</v>
       </c>
-      <c r="EF2" s="64"/>
-      <c r="EG2" s="64"/>
-      <c r="EH2" s="64"/>
-      <c r="EI2" s="65" t="s">
+      <c r="EF2" s="80"/>
+      <c r="EG2" s="80"/>
+      <c r="EH2" s="80"/>
+      <c r="EI2" s="81" t="s">
         <v>46</v>
       </c>
-      <c r="EJ2" s="65"/>
-      <c r="EK2" s="65"/>
-      <c r="EL2" s="65"/>
-      <c r="EM2" s="66" t="s">
+      <c r="EJ2" s="81"/>
+      <c r="EK2" s="81"/>
+      <c r="EL2" s="81"/>
+      <c r="EM2" s="82" t="s">
         <v>47</v>
       </c>
-      <c r="EN2" s="66"/>
-      <c r="EO2" s="66"/>
-      <c r="EP2" s="66"/>
-      <c r="EQ2" s="66"/>
-      <c r="ER2" s="66"/>
-      <c r="ES2" s="67" t="s">
+      <c r="EN2" s="82"/>
+      <c r="EO2" s="82"/>
+      <c r="EP2" s="82"/>
+      <c r="EQ2" s="82"/>
+      <c r="ER2" s="82"/>
+      <c r="ES2" s="83" t="s">
         <v>48</v>
       </c>
-      <c r="ET2" s="67"/>
-      <c r="EU2" s="67"/>
-      <c r="EV2" s="67"/>
-      <c r="EW2" s="67"/>
-      <c r="EX2" s="67"/>
-      <c r="EY2" s="67"/>
-      <c r="EZ2" s="67"/>
-      <c r="FA2" s="67"/>
-      <c r="FB2" s="67"/>
-      <c r="FC2" s="67"/>
-      <c r="FD2" s="67"/>
-      <c r="FE2" s="67"/>
-      <c r="FF2" s="67"/>
-      <c r="FG2" s="67"/>
-      <c r="FH2" s="67"/>
-      <c r="FI2" s="67"/>
-      <c r="FJ2" s="67"/>
-      <c r="FK2" s="67"/>
-      <c r="FL2" s="67"/>
-      <c r="FM2" s="67"/>
-      <c r="FN2" s="68" t="s">
+      <c r="ET2" s="83"/>
+      <c r="EU2" s="83"/>
+      <c r="EV2" s="83"/>
+      <c r="EW2" s="83"/>
+      <c r="EX2" s="83"/>
+      <c r="EY2" s="83"/>
+      <c r="EZ2" s="83"/>
+      <c r="FA2" s="83"/>
+      <c r="FB2" s="83"/>
+      <c r="FC2" s="83"/>
+      <c r="FD2" s="83"/>
+      <c r="FE2" s="83"/>
+      <c r="FF2" s="83"/>
+      <c r="FG2" s="83"/>
+      <c r="FH2" s="83"/>
+      <c r="FI2" s="83"/>
+      <c r="FJ2" s="83"/>
+      <c r="FK2" s="83"/>
+      <c r="FL2" s="83"/>
+      <c r="FM2" s="83"/>
+      <c r="FN2" s="84" t="s">
         <v>49</v>
       </c>
-      <c r="FO2" s="68"/>
-      <c r="FP2" s="68"/>
-      <c r="FQ2" s="68"/>
-      <c r="FR2" s="68"/>
-      <c r="FS2" s="68"/>
-      <c r="FT2" s="68"/>
-      <c r="FU2" s="68"/>
-      <c r="FV2" s="68"/>
-      <c r="FW2" s="68"/>
-      <c r="FX2" s="68"/>
-      <c r="FY2" s="68"/>
-      <c r="FZ2" s="68"/>
-      <c r="GA2" s="68"/>
-      <c r="GB2" s="68"/>
-      <c r="GC2" s="68"/>
-      <c r="GD2" s="68"/>
-      <c r="GE2" s="68"/>
-      <c r="GF2" s="68"/>
-      <c r="GG2" s="68"/>
-      <c r="GH2" s="68"/>
-      <c r="GI2" s="68"/>
-      <c r="GJ2" s="68"/>
-      <c r="GK2" s="68"/>
-      <c r="GL2" s="68"/>
-      <c r="GM2" s="68"/>
-      <c r="GN2" s="68"/>
-      <c r="GO2" s="68"/>
-      <c r="GP2" s="68"/>
-      <c r="GQ2" s="68"/>
-      <c r="GR2" s="68"/>
-      <c r="GS2" s="68"/>
-      <c r="GT2" s="68"/>
-      <c r="GU2" s="68"/>
-      <c r="GV2" s="68"/>
-      <c r="GW2" s="68"/>
-      <c r="GX2" s="68"/>
-      <c r="GY2" s="68"/>
-      <c r="GZ2" s="68"/>
-      <c r="HA2" s="68"/>
-      <c r="HB2" s="68"/>
-      <c r="HC2" s="68"/>
-      <c r="HD2" s="68"/>
-      <c r="HE2" s="68"/>
-      <c r="HF2" s="68"/>
-      <c r="HG2" s="68"/>
-      <c r="HH2" s="68"/>
-      <c r="HI2" s="68"/>
-      <c r="HJ2" s="68"/>
-      <c r="HK2" s="68"/>
-      <c r="HL2" s="68"/>
-      <c r="HM2" s="68"/>
-      <c r="HN2" s="68"/>
-      <c r="HO2" s="68"/>
-      <c r="HP2" s="68"/>
-      <c r="HQ2" s="68"/>
-      <c r="HR2" s="68"/>
-      <c r="HS2" s="68"/>
-      <c r="HT2" s="68"/>
-      <c r="HU2" s="68"/>
-      <c r="HV2" s="68"/>
-      <c r="HW2" s="68"/>
-      <c r="HX2" s="68"/>
-      <c r="HY2" s="68"/>
-      <c r="HZ2" s="68"/>
-      <c r="IA2" s="68"/>
-      <c r="IB2" s="68"/>
-      <c r="IC2" s="68"/>
-      <c r="ID2" s="68"/>
-      <c r="IE2" s="68"/>
-      <c r="IF2" s="68"/>
-      <c r="IG2" s="68"/>
-      <c r="IH2" s="68"/>
-      <c r="II2" s="68"/>
-      <c r="IJ2" s="68"/>
-      <c r="IK2" s="68"/>
-      <c r="IL2" s="68"/>
-      <c r="IM2" s="68"/>
-      <c r="IN2" s="68"/>
-      <c r="IO2" s="68"/>
-      <c r="IP2" s="68"/>
-      <c r="IQ2" s="68"/>
-      <c r="IR2" s="68"/>
-      <c r="IS2" s="68"/>
-      <c r="IT2" s="68"/>
-      <c r="IU2" s="68"/>
-      <c r="IV2" s="68"/>
-      <c r="IW2" s="68"/>
-      <c r="IX2" s="68"/>
-      <c r="IY2" s="68"/>
-      <c r="IZ2" s="68"/>
-      <c r="JA2" s="68"/>
-      <c r="JB2" s="68"/>
-      <c r="JC2" s="68"/>
-      <c r="JD2" s="68"/>
-      <c r="JE2" s="68"/>
-      <c r="JF2" s="68"/>
-      <c r="JG2" s="68"/>
-      <c r="JH2" s="68"/>
-      <c r="JI2" s="68"/>
-      <c r="JJ2" s="68"/>
-      <c r="JK2" s="68"/>
-      <c r="JL2" s="68"/>
-      <c r="JM2" s="68"/>
+      <c r="FO2" s="84"/>
+      <c r="FP2" s="84"/>
+      <c r="FQ2" s="84"/>
+      <c r="FR2" s="84"/>
+      <c r="FS2" s="84"/>
+      <c r="FT2" s="84"/>
+      <c r="FU2" s="84"/>
+      <c r="FV2" s="84"/>
+      <c r="FW2" s="84"/>
+      <c r="FX2" s="84"/>
+      <c r="FY2" s="84"/>
+      <c r="FZ2" s="84"/>
+      <c r="GA2" s="84"/>
+      <c r="GB2" s="84"/>
+      <c r="GC2" s="84"/>
+      <c r="GD2" s="84"/>
+      <c r="GE2" s="84"/>
+      <c r="GF2" s="84"/>
+      <c r="GG2" s="84"/>
+      <c r="GH2" s="84"/>
+      <c r="GI2" s="84"/>
+      <c r="GJ2" s="84"/>
+      <c r="GK2" s="84"/>
+      <c r="GL2" s="84"/>
+      <c r="GM2" s="84"/>
+      <c r="GN2" s="84"/>
+      <c r="GO2" s="84"/>
+      <c r="GP2" s="84"/>
+      <c r="GQ2" s="84"/>
+      <c r="GR2" s="84"/>
+      <c r="GS2" s="84"/>
+      <c r="GT2" s="84"/>
+      <c r="GU2" s="84"/>
+      <c r="GV2" s="84"/>
+      <c r="GW2" s="84"/>
+      <c r="GX2" s="84"/>
+      <c r="GY2" s="84"/>
+      <c r="GZ2" s="84"/>
+      <c r="HA2" s="84"/>
+      <c r="HB2" s="84"/>
+      <c r="HC2" s="84"/>
+      <c r="HD2" s="84"/>
+      <c r="HE2" s="84"/>
+      <c r="HF2" s="84"/>
+      <c r="HG2" s="84"/>
+      <c r="HH2" s="84"/>
+      <c r="HI2" s="84"/>
+      <c r="HJ2" s="84"/>
+      <c r="HK2" s="84"/>
+      <c r="HL2" s="84"/>
+      <c r="HM2" s="84"/>
+      <c r="HN2" s="84"/>
+      <c r="HO2" s="84"/>
+      <c r="HP2" s="84"/>
+      <c r="HQ2" s="84"/>
+      <c r="HR2" s="84"/>
+      <c r="HS2" s="84"/>
+      <c r="HT2" s="84"/>
+      <c r="HU2" s="84"/>
+      <c r="HV2" s="84"/>
+      <c r="HW2" s="84"/>
+      <c r="HX2" s="84"/>
+      <c r="HY2" s="84"/>
+      <c r="HZ2" s="84"/>
+      <c r="IA2" s="84"/>
+      <c r="IB2" s="84"/>
+      <c r="IC2" s="84"/>
+      <c r="ID2" s="84"/>
+      <c r="IE2" s="84"/>
+      <c r="IF2" s="84"/>
+      <c r="IG2" s="84"/>
+      <c r="IH2" s="84"/>
+      <c r="II2" s="84"/>
+      <c r="IJ2" s="84"/>
+      <c r="IK2" s="84"/>
+      <c r="IL2" s="84"/>
+      <c r="IM2" s="84"/>
+      <c r="IN2" s="84"/>
+      <c r="IO2" s="84"/>
+      <c r="IP2" s="84"/>
+      <c r="IQ2" s="84"/>
+      <c r="IR2" s="84"/>
+      <c r="IS2" s="84"/>
+      <c r="IT2" s="84"/>
+      <c r="IU2" s="84"/>
+      <c r="IV2" s="84"/>
+      <c r="IW2" s="84"/>
+      <c r="IX2" s="84"/>
+      <c r="IY2" s="84"/>
+      <c r="IZ2" s="84"/>
+      <c r="JA2" s="84"/>
+      <c r="JB2" s="84"/>
+      <c r="JC2" s="84"/>
+      <c r="JD2" s="84"/>
+      <c r="JE2" s="84"/>
+      <c r="JF2" s="84"/>
+      <c r="JG2" s="84"/>
+      <c r="JH2" s="84"/>
+      <c r="JI2" s="84"/>
+      <c r="JJ2" s="84"/>
+      <c r="JK2" s="84"/>
+      <c r="JL2" s="84"/>
+      <c r="JM2" s="84"/>
     </row>
     <row r="3" spans="1:273" s="4" customFormat="1" ht="80">
       <c r="A3" s="9" t="s">
@@ -7594,26 +7594,26 @@
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="EE2:EH2"/>
+    <mergeCell ref="EI2:EL2"/>
+    <mergeCell ref="EM2:ER2"/>
+    <mergeCell ref="ES2:FM2"/>
+    <mergeCell ref="FN2:JM2"/>
+    <mergeCell ref="AR2:BM2"/>
+    <mergeCell ref="BO2:CH2"/>
+    <mergeCell ref="CI2:CX2"/>
+    <mergeCell ref="CY2:DI2"/>
+    <mergeCell ref="DJ2:ED2"/>
+    <mergeCell ref="I2:U2"/>
+    <mergeCell ref="V2:AB2"/>
+    <mergeCell ref="AC2:AH2"/>
+    <mergeCell ref="AI2:AM2"/>
+    <mergeCell ref="AN2:AQ2"/>
     <mergeCell ref="A1:D1"/>
     <mergeCell ref="E1:H1"/>
     <mergeCell ref="I1:AM1"/>
     <mergeCell ref="AN1:BM1"/>
     <mergeCell ref="BN1:JM1"/>
-    <mergeCell ref="I2:U2"/>
-    <mergeCell ref="V2:AB2"/>
-    <mergeCell ref="AC2:AH2"/>
-    <mergeCell ref="AI2:AM2"/>
-    <mergeCell ref="AN2:AQ2"/>
-    <mergeCell ref="AR2:BM2"/>
-    <mergeCell ref="BO2:CH2"/>
-    <mergeCell ref="CI2:CX2"/>
-    <mergeCell ref="CY2:DI2"/>
-    <mergeCell ref="DJ2:ED2"/>
-    <mergeCell ref="EE2:EH2"/>
-    <mergeCell ref="EI2:EL2"/>
-    <mergeCell ref="EM2:ER2"/>
-    <mergeCell ref="ES2:FM2"/>
-    <mergeCell ref="FN2:JM2"/>
   </mergeCells>
   <phoneticPr fontId="14" type="noConversion"/>
   <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>